<commit_message>
Update conversion chart (spreadsheet)
</commit_message>
<xml_diff>
--- a/_workshop/conversions.xlsx
+++ b/_workshop/conversions.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmarino009\Documents\airlock\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15195" windowHeight="8445" tabRatio="854" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="48" windowWidth="15192" windowHeight="8448" tabRatio="854" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="4" r:id="rId1"/>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>nbyte0</t>
   </si>
@@ -80,9 +85,6 @@
   </si>
   <si>
     <t>TS</t>
-  </si>
-  <si>
-    <t>IN</t>
   </si>
   <si>
     <t>S</t>
@@ -157,7 +159,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,6 +187,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,9 +461,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -479,9 +484,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -496,6 +498,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="60" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,6 +593,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -619,11 +630,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="179334144"/>
-        <c:axId val="181807360"/>
+        <c:axId val="797314608"/>
+        <c:axId val="797318920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="179334144"/>
+        <c:axId val="797314608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,7 +643,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181807360"/>
+        <c:crossAx val="797318920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -640,7 +651,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181807360"/>
+        <c:axId val="797318920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -650,14 +661,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179334144"/>
+        <c:crossAx val="797314608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1033,86 +1043,86 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="Z22" sqref="Z22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="3.109375" style="1" customWidth="1"/>
     <col min="3" max="25" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="38" t="s">
+      <c r="O1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="38" t="s">
+      <c r="P1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="38" t="s">
+      <c r="Q1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="38" t="s">
+      <c r="R1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="38" t="s">
+      <c r="S1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="38" t="s">
+      <c r="T1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="38" t="s">
+      <c r="U1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="38" t="s">
+      <c r="V1" s="36" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1132,14 +1142,14 @@
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="17"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S2" s="14"/>
+      <c r="T2" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="14"/>
+      <c r="V2" s="16"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1159,14 +1169,14 @@
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
-      <c r="S3" s="16"/>
+      <c r="S3" s="15"/>
       <c r="T3" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="U3" s="16"/>
-      <c r="V3" s="18"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="U3" s="15"/>
+      <c r="V3" s="17"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1186,14 +1196,14 @@
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
-      <c r="S4" s="16"/>
+      <c r="S4" s="15"/>
       <c r="T4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="U4" s="16"/>
-      <c r="V4" s="18"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="U4" s="15"/>
+      <c r="V4" s="17"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1213,14 +1223,14 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
-      <c r="S5" s="16"/>
+      <c r="S5" s="15"/>
       <c r="T5" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="U5" s="16"/>
-      <c r="V5" s="18"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="U5" s="15"/>
+      <c r="V5" s="17"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1240,14 +1250,14 @@
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
-      <c r="S6" s="16"/>
+      <c r="S6" s="15"/>
       <c r="T6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="U6" s="16"/>
-      <c r="V6" s="18"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="U6" s="15"/>
+      <c r="V6" s="17"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1267,14 +1277,14 @@
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
-      <c r="S7" s="16"/>
+      <c r="S7" s="15"/>
       <c r="T7" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="U7" s="16"/>
-      <c r="V7" s="18"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="U7" s="15"/>
+      <c r="V7" s="17"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1294,12 +1304,12 @@
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="18"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="17"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1319,12 +1329,12 @@
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="18"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="17"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1344,12 +1354,12 @@
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="18"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="17"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1369,12 +1379,12 @@
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="18"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="17"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1394,62 +1404,62 @@
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="16"/>
-      <c r="V12" s="18"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="17"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
       <c r="N13" s="5"/>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="18"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="17"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
       <c r="N14" s="8"/>
       <c r="O14" s="5"/>
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="16"/>
-      <c r="V14" s="18"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="17"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1469,12 +1479,12 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-      <c r="U15" s="16"/>
-      <c r="V15" s="18"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="17"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
@@ -1494,12 +1504,12 @@
       <c r="P16" s="8"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="8"/>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="16"/>
-      <c r="V16" s="18"/>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="17"/>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1519,28 +1529,28 @@
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="5"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
-      <c r="V17" s="18"/>
-    </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="17"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
       <c r="P18" s="13" t="s">
         <v>20</v>
       </c>
@@ -1551,11 +1561,11 @@
         <v>20</v>
       </c>
       <c r="S18" s="5"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="18"/>
-    </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="17"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1565,175 +1575,153 @@
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
       <c r="T19" s="5"/>
-      <c r="U19" s="16"/>
-      <c r="V19" s="18"/>
-    </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="U19" s="15"/>
+      <c r="V19" s="17"/>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="40"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="Q20" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="R20" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q20" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="R20" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
       <c r="U20" s="5"/>
-      <c r="V20" s="18"/>
-    </row>
-    <row r="21" spans="2:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="V20" s="17"/>
+    </row>
+    <row r="21" spans="2:22" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
-      <c r="T21" s="20"/>
-      <c r="U21" s="20"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
       <c r="V21" s="11"/>
     </row>
-    <row r="22" spans="2:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="C23" s="23"/>
-      <c r="D23" s="24" t="s">
+    <row r="22" spans="2:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C23" s="22"/>
+      <c r="D23" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="24"/>
+      <c r="U23" s="24"/>
+      <c r="V23" s="25"/>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C24" s="26"/>
+      <c r="D24" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="25"/>
-      <c r="T23" s="25"/>
-      <c r="U23" s="25"/>
-      <c r="V23" s="26"/>
-    </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="C24" s="27"/>
-      <c r="D24" s="28" t="s">
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="29"/>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C25" s="30"/>
+      <c r="D25" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="29"/>
-      <c r="P24" s="29"/>
-      <c r="Q24" s="29"/>
-      <c r="R24" s="29"/>
-      <c r="S24" s="29"/>
-      <c r="T24" s="29"/>
-      <c r="U24" s="29"/>
-      <c r="V24" s="30"/>
-    </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="C25" s="31"/>
-      <c r="D25" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
-      <c r="Q25" s="33"/>
-      <c r="R25" s="33"/>
-      <c r="S25" s="33"/>
-      <c r="T25" s="33"/>
-      <c r="U25" s="33"/>
-      <c r="V25" s="34"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="33"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -1753,7 +1741,7 @@
   <sheetViews>
     <sheetView zoomScale="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0.2" footer="0.2"/>
@@ -1772,7 +1760,7 @@
   <sheetViews>
     <sheetView zoomScale="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0.2" footer="0.2"/>

</xml_diff>

<commit_message>
Update excel spreadsheet to show the 6 new conversions
</commit_message>
<xml_diff>
--- a/_workshop/conversions.xlsx
+++ b/_workshop/conversions.xlsx
@@ -630,11 +630,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="797314608"/>
         <c:axId val="797318920"/>
+        <c:axId val="797323232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="797314608"/>
+        <c:axId val="797318920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -643,7 +643,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="797318920"/>
+        <c:crossAx val="797323232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -651,7 +651,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="797318920"/>
+        <c:axId val="797323232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +661,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="797314608"/>
+        <c:crossAx val="797318920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1043,8 +1043,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="Z22" sqref="Z22"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1480,7 +1480,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
+      <c r="T15" s="8"/>
       <c r="U15" s="15"/>
       <c r="V15" s="17"/>
     </row>
@@ -1505,7 +1505,7 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="8"/>
       <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
+      <c r="T16" s="8"/>
       <c r="U16" s="15"/>
       <c r="V16" s="17"/>
     </row>
@@ -1530,7 +1530,7 @@
       <c r="Q17" s="8"/>
       <c r="R17" s="5"/>
       <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
+      <c r="T17" s="8"/>
       <c r="U17" s="15"/>
       <c r="V17" s="17"/>
     </row>
@@ -1582,9 +1582,9 @@
       <c r="M19" s="15"/>
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
       <c r="S19" s="15"/>
       <c r="T19" s="5"/>
       <c r="U19" s="15"/>

</xml_diff>

<commit_message>
Update conversion chart with the 9 new possible conversions
</commit_message>
<xml_diff>
--- a/_workshop/conversions.xlsx
+++ b/_workshop/conversions.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>nbyte0</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>TS</t>
-  </si>
-  <si>
-    <t>S</t>
   </si>
   <si>
     <t>C1</t>
@@ -438,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -503,6 +500,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -630,11 +632,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="797318920"/>
-        <c:axId val="797323232"/>
+        <c:axId val="726931304"/>
+        <c:axId val="726932872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="797318920"/>
+        <c:axId val="726931304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -643,7 +645,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="797323232"/>
+        <c:crossAx val="726932872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -651,7 +653,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="797323232"/>
+        <c:axId val="726932872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +663,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="797318920"/>
+        <c:crossAx val="726931304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1043,8 +1045,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="Z22" sqref="Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1056,10 +1058,10 @@
   <sheetData>
     <row r="1" spans="1:22" s="2" customFormat="1" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>32</v>
       </c>
       <c r="C1" s="36" t="s">
         <v>0</v>
@@ -1144,7 +1146,7 @@
       <c r="R2" s="9"/>
       <c r="S2" s="14"/>
       <c r="T2" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U2" s="14"/>
       <c r="V2" s="16"/>
@@ -1171,7 +1173,7 @@
       <c r="R3" s="8"/>
       <c r="S3" s="15"/>
       <c r="T3" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U3" s="15"/>
       <c r="V3" s="17"/>
@@ -1198,7 +1200,7 @@
       <c r="R4" s="8"/>
       <c r="S4" s="15"/>
       <c r="T4" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U4" s="15"/>
       <c r="V4" s="17"/>
@@ -1225,7 +1227,7 @@
       <c r="R5" s="8"/>
       <c r="S5" s="15"/>
       <c r="T5" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U5" s="15"/>
       <c r="V5" s="17"/>
@@ -1252,7 +1254,7 @@
       <c r="R6" s="8"/>
       <c r="S6" s="15"/>
       <c r="T6" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U6" s="15"/>
       <c r="V6" s="17"/>
@@ -1279,7 +1281,7 @@
       <c r="R7" s="8"/>
       <c r="S7" s="15"/>
       <c r="T7" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U7" s="15"/>
       <c r="V7" s="17"/>
@@ -1479,10 +1481,12 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
-      <c r="S15" s="15"/>
+      <c r="S15" s="44" t="s">
+        <v>20</v>
+      </c>
       <c r="T15" s="8"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="17"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="42"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -1504,10 +1508,12 @@
       <c r="P16" s="8"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="8"/>
-      <c r="S16" s="15"/>
+      <c r="S16" s="44" t="s">
+        <v>20</v>
+      </c>
       <c r="T16" s="8"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="17"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="42"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -1529,10 +1535,12 @@
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="5"/>
-      <c r="S17" s="15"/>
+      <c r="S17" s="44" t="s">
+        <v>20</v>
+      </c>
       <c r="T17" s="8"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="17"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="42"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
@@ -1607,15 +1615,9 @@
       <c r="M20" s="41"/>
       <c r="N20" s="21"/>
       <c r="O20" s="21"/>
-      <c r="P20" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q20" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="R20" s="13" t="s">
-        <v>21</v>
-      </c>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
       <c r="S20" s="15"/>
       <c r="T20" s="15"/>
       <c r="U20" s="5"/>
@@ -1638,9 +1640,9 @@
       <c r="M21" s="19"/>
       <c r="N21" s="19"/>
       <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="43"/>
       <c r="S21" s="19"/>
       <c r="T21" s="19"/>
       <c r="U21" s="19"/>
@@ -1648,13 +1650,13 @@
     </row>
     <row r="22" spans="2:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C23" s="22"/>
       <c r="D23" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
@@ -1678,7 +1680,7 @@
     <row r="24" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C24" s="26"/>
       <c r="D24" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24" s="28"/>
       <c r="F24" s="28"/>
@@ -1702,7 +1704,7 @@
     <row r="25" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C25" s="30"/>
       <c r="D25" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>

</xml_diff>